<commit_message>
Additional tests for Cell Types
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/sheet_with_all_cell_types.xlsx
+++ b/tests/resources/xlsx/sheet_with_all_cell_types.xlsx
@@ -77,6 +77,12 @@
       <c r="I1" s="0" t="e">
         <v>ERROR</v>
       </c>
+      <c r="J1" s="0" t="str">
+        <v>weird string</v>
+      </c>
+      <c r="K1" s="0" t="d">
+        <v>invalid::date</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="H2"/>

</xml_diff>